<commit_message>
adicionados os primeiros scripts
</commit_message>
<xml_diff>
--- a/Dicionario Base.xlsx
+++ b/Dicionario Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonyarrais/Documents/Universidade Federal Fluminense/Semestres/2022_1/GET00100 - Estatistica I/Trabalho Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8090ab699fe7811/Documentos/EstI_Trab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED4796B-754C-B047-9C15-522F107E2483}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1ED4796B-754C-B047-9C15-522F107E2483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08EE3E00-89EC-4D72-9709-BAD59211A153}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16140" xr2:uid="{FDE7FB03-A37C-B04D-B49B-BB85BCD408B8}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{FDE7FB03-A37C-B04D-B49B-BB85BCD408B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -556,19 +556,19 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.19921875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="29.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -603,7 +603,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -620,7 +620,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>2</v>
       </c>
@@ -628,7 +628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>3</v>
       </c>
@@ -636,7 +636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -653,7 +653,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>1</v>
       </c>
@@ -661,7 +661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -678,7 +678,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>2</v>
       </c>
@@ -686,7 +686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -700,7 +700,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -714,7 +714,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -731,7 +731,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -756,7 +756,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>1</v>
       </c>
@@ -764,7 +764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -778,7 +778,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -792,7 +792,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -806,7 +806,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -823,7 +823,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>1</v>
       </c>
@@ -831,7 +831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -848,7 +848,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>2</v>
       </c>
@@ -856,7 +856,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>3</v>
       </c>
@@ -864,7 +864,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -881,7 +881,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>1</v>
       </c>
@@ -889,7 +889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -906,7 +906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>1</v>
       </c>
@@ -914,7 +914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -931,7 +931,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>1</v>
       </c>
@@ -939,7 +939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -956,7 +956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>1</v>
       </c>
@@ -964,7 +964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
adicionado script de associação entre idade e escalas
</commit_message>
<xml_diff>
--- a/Dicionario Base.xlsx
+++ b/Dicionario Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8090ab699fe7811/Documentos/EstI_Trab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1ED4796B-754C-B047-9C15-522F107E2483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08EE3E00-89EC-4D72-9709-BAD59211A153}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{1ED4796B-754C-B047-9C15-522F107E2483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEAA256B-1CEC-4C9A-A0AB-B69721A968B7}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{FDE7FB03-A37C-B04D-B49B-BB85BCD408B8}"/>
   </bookViews>
@@ -555,14 +555,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A7ACC6-6C86-F741-8722-BB23544B5DE5}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B13" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.19921875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="67.19921875" customWidth="1"/>
     <col min="4" max="4" width="29.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.296875" style="1" bestFit="1" customWidth="1"/>

</xml_diff>